<commit_message>
gwas data sheet updated
</commit_message>
<xml_diff>
--- a/genetic data/GWAS_datasets_to_consider.xlsx
+++ b/genetic data/GWAS_datasets_to_consider.xlsx
@@ -829,10 +829,10 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="36:36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Single AD PRS Added
</commit_message>
<xml_diff>
--- a/genetic data/GWAS_datasets_to_consider.xlsx
+++ b/genetic data/GWAS_datasets_to_consider.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="139">
   <si>
     <t xml:space="preserve">GWAS_ID</t>
   </si>
@@ -431,6 +431,12 @@
   </si>
   <si>
     <t xml:space="preserve">International Parkinson's Disease Genomics Consortium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ieu-b-5067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alzheimer's disease</t>
   </si>
 </sst>
 </file>
@@ -954,9 +960,9 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2850,6 +2856,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" s="10" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="10" t="n">
+        <v>488285</v>
+      </c>
+      <c r="F54" s="10" t="n">
+        <v>12321875</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="41"/>
+      <c r="M54" s="41"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="41"/>
+      <c r="P54" s="41"/>
+      <c r="Q54" s="41"/>
+      <c r="R54" s="41"/>
+      <c r="S54" s="41"/>
+      <c r="T54" s="41"/>
+      <c r="U54" s="41"/>
+      <c r="V54" s="41"/>
+      <c r="W54" s="41"/>
+      <c r="X54" s="41"/>
+      <c r="Y54" s="41"/>
+      <c r="Z54" s="41"/>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>